<commit_message>
update cost and fp analysis
</commit_message>
<xml_diff>
--- a/FPA.xlsx
+++ b/FPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moata\source\repos\SW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F50F29-A122-4B1E-B562-6C573D956C67}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4325D60-24A6-457C-A7B8-2549F607F357}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{9804D593-F053-43A2-BA34-89D2C7CF3B29}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Weighting Factor</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Complexity weighting factor</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Backup and recovery</t>
   </si>
   <si>
@@ -193,13 +190,91 @@
   </si>
   <si>
     <t>59 LOC/FP</t>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>Value=0</t>
+  </si>
+  <si>
+    <t>Value=1</t>
+  </si>
+  <si>
+    <t>Value=2</t>
+  </si>
+  <si>
+    <t>Value=4</t>
+  </si>
+  <si>
+    <t>Value=5</t>
+  </si>
+  <si>
+    <t>Info Domain</t>
+  </si>
+  <si>
+    <t># of Inputs</t>
+  </si>
+  <si>
+    <t># of Outputs</t>
+  </si>
+  <si>
+    <t># of Inquiries</t>
+  </si>
+  <si>
+    <t># of Files</t>
+  </si>
+  <si>
+    <t>Likely</t>
+  </si>
+  <si>
+    <t>Pessimistic</t>
+  </si>
+  <si>
+    <t>Est Count</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>FP count</t>
+  </si>
+  <si>
+    <t>UFC : unadjusted Function Count</t>
+  </si>
+  <si>
+    <t>Complexity adjustment factor</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>Value=3</t>
+  </si>
+  <si>
+    <t># of External Interfaces</t>
+  </si>
+  <si>
+    <t>Optimistic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +302,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -249,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +344,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -269,7 +356,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -585,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A475971-46A1-4E59-845D-9364EE16F08F}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -598,18 +690,26 @@
     <col min="3" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
     <col min="9" max="9" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="13" width="8.6640625" style="6" customWidth="1"/>
+    <col min="14" max="15" width="8.33203125" style="6" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" style="1"/>
+    <col min="21" max="21" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="6" t="s">
+    <row r="1" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -618,13 +718,52 @@
       <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
@@ -634,19 +773,58 @@
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="9"/>
       <c r="H2" s="4">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="4">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="R2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>4</v>
+      </c>
+      <c r="U2" s="1">
+        <v>6</v>
+      </c>
+      <c r="V2" s="1">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1">
+        <v>4</v>
+      </c>
+      <c r="X2" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -657,7 +835,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <f>SUM(C3,D4:D6)</f>
         <v>15</v>
       </c>
@@ -665,14 +843,53 @@
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="4">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="R3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="1">
+        <v>8</v>
+      </c>
+      <c r="T3" s="1">
+        <v>11</v>
+      </c>
+      <c r="U3" s="1">
+        <v>14</v>
+      </c>
+      <c r="V3" s="1">
+        <v>11</v>
+      </c>
+      <c r="W3" s="1">
+        <v>5</v>
+      </c>
+      <c r="X3" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -681,19 +898,58 @@
         <v>4</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="9"/>
       <c r="H4" s="4">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="4">
+        <v>33</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="R4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="1">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>4</v>
+      </c>
+      <c r="U4" s="1">
+        <v>6</v>
+      </c>
+      <c r="V4" s="1">
+        <v>4</v>
+      </c>
+      <c r="W4" s="1">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -702,19 +958,58 @@
         <v>4</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="9"/>
       <c r="H5" s="4">
         <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>4</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>2</v>
+      </c>
+      <c r="U5" s="1">
+        <v>3</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2</v>
+      </c>
+      <c r="W5" s="1">
+        <v>10</v>
+      </c>
+      <c r="X5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -723,18 +1018,57 @@
         <v>4</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="9"/>
       <c r="H6" s="4">
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="U6" s="1">
+        <v>3</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -746,14 +1080,44 @@
         <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>4</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="1">
+        <f>SUM(X2:X6)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -764,7 +1128,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="6">
+      <c r="F8" s="9">
         <f>SUM(C8,C9,D10,E11,D12,D13,E14,D15,D16,D17,D18)</f>
         <v>57</v>
       </c>
@@ -773,14 +1137,43 @@
         <v>7</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="4">
+        <v>37</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="1">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -789,20 +1182,47 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4">
         <v>8</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="4">
+        <v>38</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="X9" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
@@ -811,20 +1231,38 @@
         <v>5</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4">
         <v>9</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="4">
+        <v>39</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
@@ -833,20 +1271,38 @@
       <c r="E11" s="4">
         <v>7</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
         <v>10</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="4">
+        <v>40</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
@@ -855,20 +1311,38 @@
         <v>5</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
         <v>11</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -877,20 +1351,38 @@
         <v>5</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4">
         <v>12</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
@@ -899,20 +1391,38 @@
       <c r="E14" s="4">
         <v>7</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4">
         <v>13</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="4">
+        <v>43</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
@@ -921,20 +1431,38 @@
         <v>5</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
         <v>14</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
@@ -943,18 +1471,24 @@
         <v>5</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="4">
-        <f>SUM(J2:J15)</f>
+        <v>45</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="4">
+        <f>SUM(P2:P15)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
@@ -963,13 +1497,19 @@
         <v>5</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -978,22 +1518,28 @@
         <v>5</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1010,58 +1556,64 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I20" s="4">
-        <v>7257</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7965</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4">
         <v>10</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="6">
+      <c r="F22" s="9">
         <f>SUM(D22:D23)</f>
         <v>20</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4">
         <v>10</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="6"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1072,14 +1624,14 @@
       <c r="E25" s="4">
         <v>10</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="9">
         <f>SUM(E25:E26)</f>
         <v>20</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1088,10 +1640,10 @@
       <c r="E26" s="4">
         <v>10</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1099,10 +1651,10 @@
       <c r="F27" s="5"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1112,19 +1664,19 @@
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F30" s="4">
-        <f>0.65+0.01*J16</f>
+        <f>0.65+0.01*P16</f>
         <v>1.06</v>
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F31" s="4">
         <v>123</v>
@@ -1132,7 +1684,9 @@
       <c r="G31" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="S7:W7"/>
+    <mergeCell ref="T8:W8"/>
     <mergeCell ref="F8:F18"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F22:F23"/>

</xml_diff>